<commit_message>
Fixed Kansas URL; moved files.
</commit_message>
<xml_diff>
--- a/NLP/entity_dictionaries/KSHS_PII__mapping.xlsx
+++ b/NLP/entity_dictionaries/KSHS_PII__mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="23040" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="23040" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>PII.ks_drivers_license_number</t>
   </si>
   <si>
-    <t>ks.gov</t>
-  </si>
-  <si>
     <t>Kansas Department of Revenue certificate of tax clearance. Taxpayers request a certificate as proof of good account standing. Tax clearance certificate includes a transaction ID and a confirmation number.</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>PII.ks_tax_clearance_certificate</t>
+  </si>
+  <si>
+    <t>kshs.org</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,10 +422,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
@@ -434,24 +434,24 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>